<commit_message>
Correção do erro para valores positivos
</commit_message>
<xml_diff>
--- a/tabelas/dados.xlsx
+++ b/tabelas/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,63 +450,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B2" t="n">
-        <v>18.74179645599539</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.741796455995388</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>17</v>
-      </c>
-      <c r="B3" t="n">
-        <v>18.33923511963249</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.339235119632491</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>24</v>
-      </c>
-      <c r="B4" t="n">
-        <v>24.26257109901654</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.2625710990165437</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>21.70597075338313</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.2059707533831308</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>23.00761720436145</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.007617204361448415</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adição de dados a planilha
</commit_message>
<xml_diff>
--- a/tabelas/dados.xlsx
+++ b/tabelas/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,18 +436,63 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Idade</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Altura</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Peso</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Gênero</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Distância real</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Distância calculada</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Erro</t>
-        </is>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.74</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.7542467618611298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adição de janela para informar a distância real
</commit_message>
<xml_diff>
--- a/tabelas/dados.xlsx
+++ b/tabelas/dados.xlsx
@@ -1,140 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
-</file>
-
-<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-  </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
-</styleSheet>
-</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -417,55 +280,4 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Idade</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Altura</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Gênero</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Distância real</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Distância calculada</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Criação da tabela novamente
</commit_message>
<xml_diff>
--- a/tabelas/dados.xlsx
+++ b/tabelas/dados.xlsx
@@ -1,3 +1,140 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+</styleSheet>
+</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -280,4 +417,129 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Idade</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Altura</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Peso</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Gênero</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Distância real</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Distância calculada</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="C2" t="n">
+        <v>83</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-2.48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="C3" t="n">
+        <v>83</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1.35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.74</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-3.07</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>